<commit_message>
made a check list for big updates
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/eri2005_missouristate_edu/Documents/RESEARCH/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA498133-DAEF-6141-ADC4-0DB0575C5A7F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BFAA364-3CE2-9048-B033-EE876BAD65E6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>apa.R</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>pages into mote package</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -503,6 +509,15 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
updating stuff trying datasets
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/eri2005_missouristate_edu/Documents/RESEARCH/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{549FBDA2-E0C9-A740-BAE7-DCB7C648A984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{B41091CC-52EF-C348-B675-4E077FADDD6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{90270FC0-A2BB-5D41-9AFD-E8EB2630728F}"/>
   <bookViews>
-    <workbookView xWindow="59200" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>apa.R</t>
   </si>
@@ -117,9 +117,6 @@
     <t>added error coding</t>
   </si>
   <si>
-    <t>overall wrapper functions</t>
-  </si>
-  <si>
     <t>checked page online</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>include data, add formula, finish example</t>
-  </si>
-  <si>
-    <t>need to fix **,  add the right screen shot</t>
   </si>
 </sst>
 </file>
@@ -492,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E338338A-298E-AF49-825D-0AFAC6B75C2C}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -511,16 +505,16 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -528,13 +522,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -542,13 +536,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -684,11 +678,6 @@
     <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated a small thing or two
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="14_{47527D8B-057E-9E49-BF9D-F0C76ED0A806}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{96A4B976-68F8-B841-B53C-E0098E86721D}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="35200" yWindow="1460" windowWidth="19200" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -657,7 +657,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
update excel, add formulas/links
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/MOTE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\MOTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="14_{47527D8B-057E-9E49-BF9D-F0C76ED0A806}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B8BDA25F-18F7-9D48-B0F4-ACE6B1A23E14}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD34D56A-787F-4495-8669-70472FD4E350}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>apa.R</t>
   </si>
@@ -129,9 +129,6 @@
     <t>http://kbroman.org/pkg_primer/pages/data.html</t>
   </si>
   <si>
-    <t>include data, add formula, finish example</t>
-  </si>
-  <si>
     <t>https://cran.r-project.org/web/packages/roxygen2/vignettes/formatting.html</t>
   </si>
   <si>
@@ -310,6 +307,21 @@
   </si>
   <si>
     <t>done rename</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>needs formula</t>
+  </si>
+  <si>
+    <t>needs formula &amp; example</t>
+  </si>
+  <si>
+    <t>needs formula, values returned, &amp; example</t>
+  </si>
+  <si>
+    <t>needs example</t>
   </si>
 </sst>
 </file>
@@ -663,44 +675,46 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A16" sqref="A16"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>93</v>
       </c>
       <c r="F1" t="s">
         <v>29</v>
       </c>
       <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
       </c>
       <c r="K1" t="s">
         <v>32</v>
@@ -714,13 +728,16 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -731,10 +748,13 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -745,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
@@ -757,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -768,10 +788,13 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -782,10 +805,13 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -796,10 +822,13 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -810,10 +839,13 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -824,10 +856,13 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="H9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -838,10 +873,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="H10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -852,10 +890,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -866,10 +907,13 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -880,10 +924,13 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -894,10 +941,13 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -908,10 +958,13 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -922,10 +975,13 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -936,10 +992,13 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -947,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
         <v>30</v>
@@ -965,7 +1024,7 @@
         <v>31</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -976,10 +1035,13 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -990,10 +1052,13 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1004,10 +1069,13 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1018,10 +1086,13 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="H22" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1032,10 +1103,13 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="H23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1046,10 +1120,13 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1060,10 +1137,13 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1071,7 +1151,10 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="H26" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1079,7 +1162,10 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="H27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1087,7 +1173,10 @@
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="H28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1095,7 +1184,10 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="H29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1103,7 +1195,10 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="H30" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
couple more edits to get into cran
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="6_{0EAE1604-8BB9-634A-8833-8C945DBFCDFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{6A22A250-B60C-664F-A74E-EE7456098040}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="6_{0EAE1604-8BB9-634A-8833-8C945DBFCDFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{0A38BBCA-300F-B044-8FF5-D722F5A4D836}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>v.chi.sq.R</t>
   </si>
   <si>
-    <t>added error coding</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -464,6 +461,9 @@
   </si>
   <si>
     <t>MOTE-shiny-page</t>
+  </si>
+  <si>
+    <t>added error coding - alpha</t>
   </si>
 </sst>
 </file>
@@ -823,16 +823,16 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="topRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
@@ -842,34 +842,34 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -877,31 +877,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -909,28 +909,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -938,19 +938,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -958,19 +958,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -978,19 +978,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -998,19 +998,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1018,19 +1018,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1038,19 +1038,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1058,19 +1058,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1078,19 +1078,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1098,19 +1098,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1118,19 +1118,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1138,19 +1138,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1158,19 +1158,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1178,19 +1178,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1198,19 +1198,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1218,19 +1218,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1238,19 +1238,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1258,19 +1258,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1278,19 +1278,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1298,19 +1298,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1318,19 +1318,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1338,19 +1338,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1358,19 +1358,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1378,19 +1378,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1398,19 +1398,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1418,19 +1418,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1438,19 +1438,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1458,19 +1458,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1493,217 +1493,217 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating dep t files
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/MOTE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebuchanan\OneDrive - Harrisburg University\RESEARCH\2 projects\MOTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="6_{0EAE1604-8BB9-634A-8833-8C945DBFCDFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{0A38BBCA-300F-B044-8FF5-D722F5A4D836}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="6_{0EAE1604-8BB9-634A-8833-8C945DBFCDFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{7F284AD2-6A87-4171-B8F4-814D2B2CCEC4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$G$30</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
   <si>
     <t>apa.R</t>
   </si>
@@ -139,81 +139,9 @@
     <t>NA</t>
   </si>
   <si>
-    <t>chiO.md</t>
-  </si>
-  <si>
-    <t>chiV.md</t>
-  </si>
-  <si>
-    <t>deptavgM.md</t>
-  </si>
-  <si>
-    <t>deptdiffM.md</t>
-  </si>
-  <si>
-    <t>deptdifft.md</t>
-  </si>
-  <si>
-    <t>deptrm.md</t>
-  </si>
-  <si>
-    <t>epsilon.md</t>
-  </si>
-  <si>
-    <t>etaf.md</t>
-  </si>
-  <si>
-    <t>etafull.md</t>
-  </si>
-  <si>
-    <t>etapart.md</t>
-  </si>
-  <si>
-    <t>gespart.md</t>
-  </si>
-  <si>
-    <t>GOSRM.md</t>
-  </si>
-  <si>
-    <t>independentproportions.md</t>
-  </si>
-  <si>
-    <t>indtd.md</t>
-  </si>
-  <si>
-    <t>indtm.md</t>
-  </si>
-  <si>
-    <t>indtt.md</t>
-  </si>
-  <si>
-    <t>omegaf.md</t>
-  </si>
-  <si>
-    <t>OmegapartialBN.md</t>
-  </si>
-  <si>
-    <t>OmegaSS.md</t>
-  </si>
-  <si>
-    <t>singlesampletmeans.md</t>
-  </si>
-  <si>
-    <t>singlett.md</t>
-  </si>
-  <si>
-    <t>ztestmeans.md</t>
-  </si>
-  <si>
-    <t>ztestz.md</t>
-  </si>
-  <si>
     <t>page file name</t>
   </si>
   <si>
-    <t>rename</t>
-  </si>
-  <si>
     <t>dtor</t>
   </si>
   <si>
@@ -301,9 +229,6 @@
     <t>R file name</t>
   </si>
   <si>
-    <t>done rename</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -313,21 +238,6 @@
     <t>needs example</t>
   </si>
   <si>
-    <t>dtor.md</t>
-  </si>
-  <si>
-    <t>gindt.md</t>
-  </si>
-  <si>
-    <t>rcorrel.md</t>
-  </si>
-  <si>
-    <t>gesmixss.md</t>
-  </si>
-  <si>
-    <t>omegaprmss.md</t>
-  </si>
-  <si>
     <t>enhancement</t>
   </si>
   <si>
@@ -464,6 +374,15 @@
   </si>
   <si>
     <t>added error coding - alpha</t>
+  </si>
+  <si>
+    <t>add stop and alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add estimate, stats, item, fix mbess, </t>
+  </si>
+  <si>
+    <t>checked</t>
   </si>
 </sst>
 </file>
@@ -483,12 +402,18 @@
       <name val="HelveticaNeue"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -503,9 +428,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,59 +746,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E338338A-298E-AF49-825D-0AFAC6B75C2C}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+      <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -883,117 +803,108 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1001,19 +912,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1021,19 +926,19 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>116</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1041,19 +946,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1061,19 +960,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1081,19 +974,13 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1101,19 +988,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1121,19 +1002,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1141,19 +1016,13 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1161,19 +1030,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1181,19 +1044,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1201,19 +1058,13 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1221,19 +1072,13 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>53</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1241,19 +1086,13 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1261,19 +1100,13 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1281,19 +1114,13 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>56</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1301,19 +1128,13 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1321,19 +1142,13 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1341,19 +1156,13 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>59</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1361,19 +1170,13 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1381,19 +1184,13 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>61</v>
+      </c>
+      <c r="G26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1401,19 +1198,13 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>62</v>
+      </c>
+      <c r="G27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1421,19 +1212,13 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-      <c r="I28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>63</v>
+      </c>
+      <c r="G28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1441,19 +1226,13 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1461,20 +1240,14 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L30">
+  <sortState ref="A2:J30">
     <sortCondition ref="A2:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1489,221 +1262,221 @@
       <selection sqref="A1:A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated stuff and things
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\MOTE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA2786D-99A1-4E76-AABC-37660D2E0FDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="6_{26CA0726-1014-B048-9F0D-5AAD8ADFDBCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{99EB00C6-BF8E-6042-91B9-512111D7405F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$30</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="102">
   <si>
     <t>apa.R</t>
   </si>
@@ -229,9 +229,6 @@
     <t>R file name</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>needs formula &amp; example</t>
   </si>
   <si>
@@ -241,135 +238,6 @@
     <t>enhancement</t>
   </si>
   <si>
-    <t>$statistic which is the test statistic</t>
-  </si>
-  <si>
-    <t>$estimate is the effect size and CI</t>
-  </si>
-  <si>
-    <t>$full result is both </t>
-  </si>
-  <si>
-    <t>$estimate</t>
-  </si>
-  <si>
-    <t>$estimate$Intercept</t>
-  </si>
-  <si>
-    <t>[1] "$b = 37.88$, 95\\% CI $[33.65$, $42.12]$"</t>
-  </si>
-  <si>
-    <t>$estimate$cyl</t>
-  </si>
-  <si>
-    <t>[1] "$b = -2.88$, 95\\% CI $[-3.53$, $-2.22]$"</t>
-  </si>
-  <si>
-    <t>$estimate$modelfit</t>
-  </si>
-  <si>
-    <t>$estimate$modelfit$r2</t>
-  </si>
-  <si>
-    <t>[1] "$R^2 = .73$, 90\\% CI $[0.55$, $0.84]$"</t>
-  </si>
-  <si>
-    <t>$estimate$modelfit$r2_adj</t>
-  </si>
-  <si>
-    <t>[1] "$R^2_{adj} = .72$"</t>
-  </si>
-  <si>
-    <t>$estimate$modelfit$aic</t>
-  </si>
-  <si>
-    <t>[1] "$\\mathrm{AIC} = 169.31$"</t>
-  </si>
-  <si>
-    <t>$estimate$modelfit$bic</t>
-  </si>
-  <si>
-    <t>[1] "$\\mathrm{BIC} = 173.70$"</t>
-  </si>
-  <si>
-    <t>$statistic</t>
-  </si>
-  <si>
-    <t>$statistic$Intercept</t>
-  </si>
-  <si>
-    <t>[1] "$t(30) = 18.27$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$statistic$cyl</t>
-  </si>
-  <si>
-    <t>[1] "$t(30) = -8.92$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$statistic$modelfit</t>
-  </si>
-  <si>
-    <t>$statistic$modelfit$r2</t>
-  </si>
-  <si>
-    <t>[1] "$F(1, 30) = 79.56$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$full_result</t>
-  </si>
-  <si>
-    <t>$full_result$Intercept</t>
-  </si>
-  <si>
-    <t>[1] "$b = 37.88$, 95\\% CI $[33.65$, $42.12]$, $t(30) = 18.27$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$full_result$cyl</t>
-  </si>
-  <si>
-    <t>[1] "$b = -2.88$, 95\\% CI $[-3.53$, $-2.22]$, $t(30) = -8.92$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$full_result$modelfit</t>
-  </si>
-  <si>
-    <t>$full_result$modelfit$r2</t>
-  </si>
-  <si>
-    <t>[1] "$R^2 = .73$, 90\\% CI $[0.55$, $0.84]$, $F(1, 30) = 79.56$, $p &lt; .001$"</t>
-  </si>
-  <si>
-    <t>$table</t>
-  </si>
-  <si>
-    <t>A data.frame with 5 labelled columns:</t>
-  </si>
-  <si>
-    <t>  predictor estimate                 ci statistic p.value</t>
-  </si>
-  <si>
-    <t>1 Intercept    37.88 $[33.65$, $42.12]$     18.27  &lt; .001</t>
-  </si>
-  <si>
-    <t>2       Cyl    -2.88 $[-3.53$, $-2.22]$     -8.92  &lt; .001</t>
-  </si>
-  <si>
-    <t>predictor: Predictor </t>
-  </si>
-  <si>
-    <t>estimate : $b$ </t>
-  </si>
-  <si>
-    <t>ci       : 95\% CI </t>
-  </si>
-  <si>
-    <t>statistic: $t(30)$ </t>
-  </si>
-  <si>
-    <t>p.value  : $p$ </t>
-  </si>
-  <si>
     <t>added error coding - alpha</t>
   </si>
   <si>
@@ -419,13 +287,61 @@
   </si>
   <si>
     <t>need to check example formula &amp; add correct mote screenshot</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>items include estimate/statistic</t>
+  </si>
+  <si>
+    <t>import is correct with mbess</t>
+  </si>
+  <si>
+    <t>example is correct</t>
+  </si>
+  <si>
+    <t>function includes missing and checks</t>
+  </si>
+  <si>
+    <t>output includes estimate</t>
+  </si>
+  <si>
+    <t>bottom is correct</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>looks good to me</t>
+  </si>
+  <si>
+    <t>I updated MOTE because it was not showing summary statistics - can you update the webpage with the summary statistics thing and the graphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you can totally use the example here for IND t as the example for d to r (and on the mote page too), but you will need to change the example to IND t not DEP t (pictures are ok they are already IND t). </t>
+  </si>
+  <si>
+    <t>see notes on the shiny page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could probably modify the example from the z- score page just create means with the same z-score. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there's an example here - let's use it for the MOTE help page. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on this page, there's two formulas for d, only use the first one. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -437,8 +353,14 @@
       <color rgb="FF000000"/>
       <name val="HelveticaNeue"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPSMT"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +379,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -470,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -480,6 +408,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,24 +728,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E338338A-298E-AF49-825D-0AFAC6B75C2C}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="G29" sqref="G29"/>
+    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="27.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="6" max="7" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -825,16 +758,16 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="H1" t="s">
         <v>33</v>
@@ -872,7 +805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60">
+    <row r="3" spans="1:11" ht="85">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -889,16 +822,16 @@
         <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="85">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -915,14 +848,14 @@
         <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="60">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="68">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -939,14 +872,14 @@
         <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="90">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="102">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -963,14 +896,14 @@
         <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="51">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -987,14 +920,14 @@
         <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="85">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1011,14 +944,14 @@
         <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="51">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1035,14 +968,14 @@
         <v>29</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="90">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="102">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1059,165 +992,256 @@
         <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>114</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="85">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="119">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H16" t="s">
-        <v>68</v>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="68">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="51">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="G21" t="s">
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="H23" t="s">
         <v>67</v>
@@ -1225,148 +1249,117 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>82</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="H30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" t="s">
-        <v>126</v>
-      </c>
-      <c r="H31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-      <c r="H32" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K32">
-    <sortCondition ref="A2:A32"/>
+  <sortState ref="A2:K30">
+    <sortCondition ref="A2:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1374,228 +1367,553 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection sqref="A1:A65"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.5" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7" ht="68">
       <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>90</v>
       </c>
+      <c r="F1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34">
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34">
+      <c r="A14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34">
+      <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34">
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A33" s="1"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A36" s="1"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A37" s="1"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A43" s="1"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A46" s="1"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="A50" s="1"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="A55" s="1"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I belive I fixed this nonsense
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="27" documentId="6_{26CA0726-1014-B048-9F0D-5AAD8ADFDBCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{99EB00C6-BF8E-6042-91B9-512111D7405F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -730,9 +730,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E338338A-298E-AF49-825D-0AFAC6B75C2C}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD20"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -1369,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="261" zoomScaleNormal="261" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some updates before I leave the library
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\MOTE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Research/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{31598F87-EA82-2F48-91E1-75CE7ACC66BB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$2:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="103">
   <si>
     <t>apa.R</t>
   </si>
@@ -323,6 +323,21 @@
   </si>
   <si>
     <t>wrong example text, should be sports, redo JASP pic</t>
+  </si>
+  <si>
+    <t>this app page isn't working</t>
+  </si>
+  <si>
+    <t>MOTE CRAN</t>
+  </si>
+  <si>
+    <t>website page name</t>
+  </si>
+  <si>
+    <t>shiny page</t>
+  </si>
+  <si>
+    <t>MOTE Shiny + Webpage</t>
   </si>
 </sst>
 </file>
@@ -348,7 +363,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +378,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F669E"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -380,15 +401,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -396,12 +415,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7F669E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -709,24 +741,876 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19" style="4"/>
+    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="6"/>
+      <c r="B1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="34">
+      <c r="A2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="17">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="17">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="17">
+      <c r="A6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="17">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="17">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="17">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="17">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="17">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="68">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17">
+      <c r="A13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="85">
+      <c r="A14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="34">
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34">
+      <c r="A16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17">
+      <c r="A19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17">
+      <c r="A20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17">
+      <c r="A21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17">
+      <c r="A22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17">
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17">
+      <c r="A26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17">
+      <c r="A27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17">
+      <c r="A28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E338338A-298E-AF49-825D-0AFAC6B75C2C}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="27.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="6" max="7" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -803,7 +1687,7 @@
       <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>70</v>
@@ -825,7 +1709,7 @@
       <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3"/>
       <c r="H4" s="2" t="s">
         <v>70</v>
@@ -847,7 +1731,7 @@
       <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>70</v>
@@ -869,7 +1753,7 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>70</v>
@@ -891,7 +1775,7 @@
       <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="3"/>
       <c r="H7" s="2" t="s">
         <v>70</v>
@@ -913,7 +1797,7 @@
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
         <v>70</v>
@@ -935,7 +1819,7 @@
       <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
         <v>70</v>
@@ -957,7 +1841,7 @@
       <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
         <v>70</v>
@@ -979,13 +1863,13 @@
       <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="75">
+    <row r="12" spans="1:11" ht="85">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1025,13 +1909,13 @@
       <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="105">
+    <row r="14" spans="1:11" ht="119">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1939,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="60">
+    <row r="15" spans="1:11" ht="68">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30">
+    <row r="16" spans="1:11" ht="51">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,7 +1987,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="17">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1112,6 +1996,9 @@
       </c>
       <c r="C17" t="s">
         <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="H17" t="s">
         <v>67</v>
@@ -1353,564 +2240,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K30">
+  <sortState ref="A2:K30">
     <sortCondition ref="A2:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
-  <dimension ref="A1:G65"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="261" zoomScaleNormal="261" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.44140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="60">
-      <c r="A1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30">
-      <c r="A14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed all the package things!
until i see the next typo
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Research/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4787AB14-6462-0A45-818A-9000E1C5CD7C}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2A5E6AD2-F52B-9C46-B3A7-764BB6553C83}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="14400" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="99">
   <si>
     <t>apa.R</t>
   </si>
@@ -305,18 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">on this page, there's two formulas for d, only use the first one. </t>
-  </si>
-  <si>
-    <t>dept_data</t>
-  </si>
-  <si>
-    <t>ind_data</t>
-  </si>
-  <si>
-    <t>bn1_data</t>
-  </si>
-  <si>
-    <t>singt_data</t>
   </si>
   <si>
     <t>check reference</t>
@@ -744,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16"/>
@@ -758,7 +746,7 @@
     <row r="1" spans="1:9">
       <c r="A1" s="6"/>
       <c r="B1" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -766,7 +754,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I1" s="9"/>
     </row>
@@ -793,10 +781,10 @@
         <v>83</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17">
@@ -1211,7 +1199,7 @@
         <v>51</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17">
@@ -1350,16 +1338,28 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="17">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="B23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H23" s="6" t="s">
         <v>58</v>
       </c>
@@ -1374,7 +1374,9 @@
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E24" s="5" t="s">
         <v>84</v>
       </c>
@@ -1401,7 +1403,9 @@
       <c r="C25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1425,7 +1429,9 @@
       <c r="C26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E26" s="5" t="s">
         <v>84</v>
       </c>
@@ -1452,7 +1458,9 @@
       <c r="C27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E27" s="5" t="s">
         <v>84</v>
       </c>
@@ -1466,7 +1474,7 @@
         <v>62</v>
       </c>
       <c r="I27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17">
@@ -1479,7 +1487,9 @@
       <c r="C28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>84</v>
       </c>
@@ -1496,16 +1506,28 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="17">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="B29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H29" s="6" t="s">
         <v>38</v>
       </c>
@@ -1513,16 +1535,28 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="17">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="B30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H30" s="6" t="s">
         <v>64</v>
       </c>
@@ -1613,8 +1647,8 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -2014,7 +2048,7 @@
         <v>51</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
         <v>67</v>
@@ -2169,7 +2203,7 @@
         <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H27" t="s">
         <v>67</v>
@@ -2224,35 +2258,23 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" t="s">
+      <c r="H31" t="s">
         <v>92</v>
       </c>
-      <c r="H31" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
       <c r="H32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8">
       <c r="H33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8">
       <c r="H34" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
going to go through shiny and such next
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Research/2 projects/MOTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2A5E6AD2-F52B-9C46-B3A7-764BB6553C83}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{777DC3CF-96A3-4C4A-9202-927E2204BD6F}"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="14400" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="100">
   <si>
     <t>apa.R</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>MOTE Shiny + Webpage</t>
+  </si>
+  <si>
+    <t>website page</t>
   </si>
 </sst>
 </file>
@@ -730,20 +733,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="19" style="4"/>
-    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="6"/>
       <c r="B1" s="10" t="s">
         <v>95</v>
@@ -757,8 +761,9 @@
         <v>98</v>
       </c>
       <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="34">
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="34">
       <c r="A2" s="7" t="s">
         <v>77</v>
       </c>
@@ -784,10 +789,13 @@
         <v>96</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:10" ht="17">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -812,9 +820,10 @@
       <c r="H3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="17">
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="17">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -839,9 +848,10 @@
       <c r="H4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="17">
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="17">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -866,9 +876,10 @@
       <c r="H5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="17">
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="17">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -893,9 +904,10 @@
       <c r="H6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="17">
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="17">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -920,9 +932,10 @@
       <c r="H7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="17">
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="17">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -947,9 +960,10 @@
       <c r="H8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="17">
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="17">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -974,9 +988,10 @@
       <c r="H9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="17">
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="17">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1001,9 +1016,10 @@
       <c r="H10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="17">
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="17">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1029,8 +1045,9 @@
         <v>45</v>
       </c>
       <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="68">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="68">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -1055,11 +1072,12 @@
       <c r="H12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17">
+    <row r="13" spans="1:10" ht="17">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -1085,8 +1103,9 @@
         <v>47</v>
       </c>
       <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="85">
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="85">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -1111,11 +1130,12 @@
       <c r="H14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="34">
+    <row r="15" spans="1:10" ht="34">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1140,11 +1160,12 @@
       <c r="H15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="6"/>
+      <c r="J15" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="34">
+    <row r="16" spans="1:10" ht="34">
       <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1169,11 +1190,12 @@
       <c r="H16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="6"/>
+      <c r="J16" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17">
+    <row r="17" spans="1:10" ht="17">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
@@ -1198,11 +1220,12 @@
       <c r="H17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="6"/>
+      <c r="J17" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17">
+    <row r="18" spans="1:10" ht="17">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1227,8 +1250,9 @@
       <c r="H18" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="17">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="17">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
@@ -1253,8 +1277,9 @@
       <c r="H19" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="17">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="17">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1279,8 +1304,9 @@
       <c r="H20" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="17">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="17">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1305,11 +1331,12 @@
       <c r="H21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="6"/>
+      <c r="J21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17">
+    <row r="22" spans="1:10" ht="17">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1334,11 +1361,12 @@
       <c r="H22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="6"/>
+      <c r="J22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17">
+    <row r="23" spans="1:10" ht="17">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1363,8 +1391,9 @@
       <c r="H23" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="17">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="17">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1389,11 +1418,12 @@
       <c r="H24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="6"/>
+      <c r="J24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17">
+    <row r="25" spans="1:10" ht="17">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1418,8 +1448,9 @@
       <c r="H25" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="17">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="17">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1444,11 +1475,12 @@
       <c r="H26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="6"/>
+      <c r="J26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17">
+    <row r="27" spans="1:10" ht="17">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1473,11 +1505,12 @@
       <c r="H27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="6"/>
+      <c r="J27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17">
+    <row r="28" spans="1:10" ht="17">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1502,11 +1535,12 @@
       <c r="H28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="6"/>
+      <c r="J28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17">
+    <row r="29" spans="1:10" ht="17">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -1531,11 +1565,12 @@
       <c r="H29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="6"/>
+      <c r="J29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17">
+    <row r="30" spans="1:10" ht="17">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1560,8 +1595,9 @@
       <c r="H30" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1"/>
     </row>
     <row r="33" spans="1:1">
@@ -1636,7 +1672,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>